<commit_message>
Added log rank calculations
</commit_message>
<xml_diff>
--- a/bin/Tables.xlsx
+++ b/bin/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\survival-models\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88FA5AE-D708-41C7-8F15-254164FF928F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E947D560-631E-4559-90A8-19F10B0E75FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12690" windowHeight="11280" activeTab="1" xr2:uid="{C3929536-6DEA-4134-862E-CBCA1F30A99D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Table 2.2" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2.10" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Time</t>
   </si>
@@ -231,11 +231,55 @@
       <t>i</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                     </t>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1i</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +354,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,13 +388,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1561927</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>66624</xdr:rowOff>
@@ -878,10 +935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9D7155-2D81-4371-B675-557760D0E58A}">
-  <dimension ref="B2:J15"/>
+  <dimension ref="B2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,17 +946,18 @@
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="8" width="7" style="5" customWidth="1"/>
     <col min="9" max="9" width="20" style="5" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="10" max="10" width="10.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
@@ -907,7 +965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
@@ -915,8 +973,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,12 +996,15 @@
       <c r="H7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -968,11 +1029,14 @@
       <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="10">
+        <v>-0.55600000000000005</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>14</v>
       </c>
@@ -997,11 +1061,14 @@
       <c r="I10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>44</v>
       </c>
@@ -1026,11 +1093,14 @@
       <c r="I11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="10">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>98</v>
       </c>
@@ -1055,11 +1125,14 @@
       <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>104</v>
       </c>
@@ -1084,11 +1157,14 @@
       <c r="I13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>114</v>
       </c>
@@ -1113,14 +1189,49 @@
       <c r="I14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="J16" s="11">
+        <f>SUM(J9:J14)</f>
+        <v>0.748</v>
+      </c>
+      <c r="K16" s="11">
+        <f>0.2469+0.2344+0.2449+0.3333+0.25+0</f>
+        <v>1.3094999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="11"/>
+      <c r="K17" s="13">
+        <f>J16^2/K16</f>
+        <v>0.4272653684612448</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>